<commit_message>
now is working the colums D-F and lines 25-40
</commit_message>
<xml_diff>
--- a/cotizacion.xlsx
+++ b/cotizacion.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t xml:space="preserve">Cotización </t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">CONECTOR MC4 CAL 4mm (1 HEMBRA, 1 MACHO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INVERSOR GROWATT MIN 3600 TLX</t>
   </si>
   <si>
     <t xml:space="preserve">PANEL FOTOVOLTAICO 585 W MARCA CANADIAN SOLAR O SIMILAR</t>
@@ -1352,9 +1349,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675360</xdr:colOff>
       <xdr:row>314</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1367,8 +1364,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1563840" y="57903120"/>
-          <a:ext cx="10150920" cy="348120"/>
+          <a:off x="1564560" y="57903120"/>
+          <a:ext cx="10150200" cy="347400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1389,9 +1386,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675360</xdr:colOff>
       <xdr:row>362</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1404,8 +1401,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1563840" y="66780360"/>
-          <a:ext cx="10150920" cy="348480"/>
+          <a:off x="1564560" y="66780360"/>
+          <a:ext cx="10150200" cy="347760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1426,9 +1423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675360</xdr:colOff>
       <xdr:row>410</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1441,8 +1438,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1563840" y="75638880"/>
-          <a:ext cx="10150920" cy="348120"/>
+          <a:off x="1564560" y="75638880"/>
+          <a:ext cx="10150200" cy="347400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1463,9 +1460,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675360</xdr:colOff>
       <xdr:row>458</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1478,8 +1475,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1563840" y="84430440"/>
-          <a:ext cx="10150920" cy="348120"/>
+          <a:off x="1564560" y="84430440"/>
+          <a:ext cx="10150200" cy="347400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1500,9 +1497,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>682200</xdr:colOff>
+      <xdr:colOff>681480</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>327960</xdr:rowOff>
+      <xdr:rowOff>327240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1515,8 +1512,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1148040" y="22307400"/>
-          <a:ext cx="1455840" cy="499680"/>
+          <a:off x="1148760" y="22307400"/>
+          <a:ext cx="1454760" cy="498960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1537,9 +1534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>682200</xdr:colOff>
+      <xdr:colOff>681480</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>327960</xdr:rowOff>
+      <xdr:rowOff>327240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1552,8 +1549,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1148040" y="31204080"/>
-          <a:ext cx="1455840" cy="499320"/>
+          <a:off x="1148760" y="31204080"/>
+          <a:ext cx="1454760" cy="498600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1574,9 +1571,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>682200</xdr:colOff>
+      <xdr:colOff>681480</xdr:colOff>
       <xdr:row>218</xdr:row>
-      <xdr:rowOff>327960</xdr:rowOff>
+      <xdr:rowOff>327240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1589,8 +1586,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1148040" y="40081320"/>
-          <a:ext cx="1455840" cy="499320"/>
+          <a:off x="1148760" y="40081320"/>
+          <a:ext cx="1454760" cy="498600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,9 +1608,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>682200</xdr:colOff>
+      <xdr:colOff>681480</xdr:colOff>
       <xdr:row>266</xdr:row>
-      <xdr:rowOff>327960</xdr:rowOff>
+      <xdr:rowOff>327240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1626,8 +1623,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1148040" y="48967920"/>
-          <a:ext cx="1455840" cy="499680"/>
+          <a:off x="1148760" y="48967920"/>
+          <a:ext cx="1454760" cy="498960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1650,10 +1647,10 @@
   <dimension ref="B2:O505"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.7"/>
@@ -2213,7 +2210,7 @@
       <c r="B33" s="22"/>
       <c r="C33" s="33"/>
       <c r="D33" s="40" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>38</v>
@@ -2230,15 +2227,9 @@
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="22"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="40" t="n">
-        <v>8</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>47</v>
-      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="46"/>
       <c r="G34" s="46"/>
       <c r="H34" s="46"/>
       <c r="I34" s="46"/>
@@ -2260,10 +2251,10 @@
         <v>1</v>
       </c>
       <c r="E36" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="48" t="s">
         <v>48</v>
-      </c>
-      <c r="F36" s="48" t="s">
-        <v>49</v>
       </c>
       <c r="G36" s="48"/>
       <c r="H36" s="48"/>
@@ -2279,10 +2270,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G37" s="43"/>
       <c r="H37" s="43"/>
@@ -2301,7 +2292,7 @@
         <v>38</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G38" s="48"/>
       <c r="H38" s="48"/>
@@ -2320,7 +2311,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -2339,7 +2330,7 @@
         <v>33</v>
       </c>
       <c r="F40" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G40" s="48"/>
       <c r="H40" s="48"/>
@@ -2401,7 +2392,7 @@
       <c r="B46" s="22"/>
       <c r="C46" s="33"/>
       <c r="F46" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G46" s="51"/>
       <c r="H46" s="51"/>
@@ -2431,7 +2422,7 @@
       <c r="D48" s="37"/>
       <c r="E48" s="52"/>
       <c r="F48" s="53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G48" s="53"/>
       <c r="H48" s="53"/>
@@ -2484,7 +2475,7 @@
     <row r="52" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="60"/>
       <c r="C52" s="61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="61"/>
       <c r="E52" s="61"/>
@@ -2493,20 +2484,20 @@
       <c r="H52" s="61"/>
       <c r="I52" s="61"/>
       <c r="J52" s="62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K52" s="63" t="n">
         <f aca="false">K19</f>
         <v>84482</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="60"/>
       <c r="C53" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D53" s="64"/>
       <c r="E53" s="64"/>
@@ -2515,20 +2506,20 @@
       <c r="H53" s="64"/>
       <c r="I53" s="64"/>
       <c r="J53" s="65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K53" s="66" t="n">
         <f aca="false">K52*0.16</f>
         <v>13517.12</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="60"/>
       <c r="C54" s="64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D54" s="64"/>
       <c r="E54" s="64"/>
@@ -2537,20 +2528,20 @@
       <c r="H54" s="64"/>
       <c r="I54" s="64"/>
       <c r="J54" s="65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K54" s="67" t="n">
         <f aca="false">SUM(K52:K53)</f>
         <v>97999.12</v>
       </c>
       <c r="L54" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="60"/>
       <c r="C55" s="64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="64"/>
       <c r="E55" s="64"/>
@@ -2565,7 +2556,7 @@
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="60"/>
       <c r="C56" s="61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D56" s="61"/>
       <c r="E56" s="61"/>
@@ -2580,7 +2571,7 @@
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="60"/>
       <c r="C57" s="61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D57" s="61"/>
       <c r="E57" s="61"/>
@@ -2609,7 +2600,7 @@
       <c r="B59" s="60"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E59" s="71"/>
       <c r="F59" s="71"/>
@@ -2703,7 +2694,7 @@
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="60"/>
       <c r="C66" s="73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D66" s="73"/>
       <c r="E66" s="73"/>

</xml_diff>

<commit_message>
solved 2 decimals problem
</commit_message>
<xml_diff>
--- a/cotizacion.xlsx
+++ b/cotizacion.xlsx
@@ -1353,9 +1353,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>675000</xdr:colOff>
+      <xdr:colOff>674280</xdr:colOff>
       <xdr:row>314</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1369,7 +1369,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="57903120"/>
-          <a:ext cx="10149840" cy="347040"/>
+          <a:ext cx="10149120" cy="346320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1390,9 +1390,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>675000</xdr:colOff>
+      <xdr:colOff>674280</xdr:colOff>
       <xdr:row>362</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1406,7 +1406,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="66780360"/>
-          <a:ext cx="10149840" cy="347400"/>
+          <a:ext cx="10149120" cy="346680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1427,9 +1427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>675000</xdr:colOff>
+      <xdr:colOff>674280</xdr:colOff>
       <xdr:row>410</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1443,7 +1443,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="75638880"/>
-          <a:ext cx="10149840" cy="347040"/>
+          <a:ext cx="10149120" cy="346320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1464,9 +1464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>675000</xdr:colOff>
+      <xdr:colOff>674280</xdr:colOff>
       <xdr:row>458</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1480,7 +1480,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="84430440"/>
-          <a:ext cx="10149840" cy="347040"/>
+          <a:ext cx="10149120" cy="346320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1501,9 +1501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>681120</xdr:colOff>
+      <xdr:colOff>680400</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>326880</xdr:rowOff>
+      <xdr:rowOff>326160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1517,7 +1517,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="22307400"/>
-          <a:ext cx="1454400" cy="498600"/>
+          <a:ext cx="1453680" cy="497880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1538,9 +1538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>681120</xdr:colOff>
+      <xdr:colOff>680400</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>326880</xdr:rowOff>
+      <xdr:rowOff>326160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1554,7 +1554,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="31204080"/>
-          <a:ext cx="1454400" cy="498240"/>
+          <a:ext cx="1453680" cy="497520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1575,9 +1575,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>681120</xdr:colOff>
+      <xdr:colOff>680400</xdr:colOff>
       <xdr:row>218</xdr:row>
-      <xdr:rowOff>326880</xdr:rowOff>
+      <xdr:rowOff>326160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1591,7 +1591,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="40081320"/>
-          <a:ext cx="1454400" cy="498240"/>
+          <a:ext cx="1453680" cy="497520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1612,9 +1612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>681120</xdr:colOff>
+      <xdr:colOff>680400</xdr:colOff>
       <xdr:row>266</xdr:row>
-      <xdr:rowOff>326880</xdr:rowOff>
+      <xdr:rowOff>326160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1628,7 +1628,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="48967920"/>
-          <a:ext cx="1454400" cy="498600"/>
+          <a:ext cx="1453680" cy="497880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1650,8 +1650,8 @@
   </sheetPr>
   <dimension ref="B2:O505"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K38" activeCellId="0" sqref="K38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K52" activeCellId="0" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1988,11 +1988,11 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
       <c r="J19" s="36" t="n">
-        <v>84482</v>
+        <v>84482.75</v>
       </c>
       <c r="K19" s="36" t="n">
         <f aca="false">J19</f>
-        <v>84482</v>
+        <v>84482.75</v>
       </c>
       <c r="L19" s="36"/>
     </row>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="K52" s="63" t="n">
         <f aca="false">K19</f>
-        <v>84482</v>
+        <v>84482.75</v>
       </c>
       <c r="L52" s="13" t="s">
         <v>57</v>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="K53" s="66" t="n">
         <f aca="false">K52*0.16</f>
-        <v>13517.12</v>
+        <v>13517.24</v>
       </c>
       <c r="L53" s="13" t="s">
         <v>57</v>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="K54" s="67" t="n">
         <f aca="false">SUM(K52:K53)</f>
-        <v>97999.12</v>
+        <v>97999.99</v>
       </c>
       <c r="L54" s="13" t="s">
         <v>57</v>

</xml_diff>